<commit_message>
Add Automation for SQL Server and Web Scraping
</commit_message>
<xml_diff>
--- a/homologación/productos.xlsx
+++ b/homologación/productos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpiscoya\Desktop\Automatización\Homologación Productos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpiscoya\OneDrive - Laive\Documentos\python-projects\homologación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670933A1-4224-45A0-871F-BFCA5B7C70D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72800F1-48CD-4D3E-962D-04E9134DBB76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{62428D55-77F9-4330-ADC7-D593BE507B78}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>DEX</t>
   </si>
@@ -53,32 +53,68 @@
     <t>PESO</t>
   </si>
   <si>
-    <t>50001227</t>
-  </si>
-  <si>
     <t>CENCOSUD</t>
   </si>
   <si>
-    <t>1029712</t>
-  </si>
-  <si>
-    <t>TWOPACK BEB ALMENDRA SIN END LAIVE 946ML</t>
-  </si>
-  <si>
-    <t>80000153</t>
-  </si>
-  <si>
-    <t>1029715</t>
-  </si>
-  <si>
-    <t>"SIROPE SABOR A MAPLE LAIVE X 750 ML"</t>
+    <t>DIJISA</t>
+  </si>
+  <si>
+    <t>484329005</t>
+  </si>
+  <si>
+    <t>YOGURT GRIEGO LAIVE ORIGINAL ENDULZADO</t>
+  </si>
+  <si>
+    <t>80000156</t>
+  </si>
+  <si>
+    <t>Daro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80000156       </t>
+  </si>
+  <si>
+    <t>BISCOLATA VENITRIO CREM AVELL 20G/24U/6D</t>
+  </si>
+  <si>
+    <t>80000157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80000157       </t>
+  </si>
+  <si>
+    <t>WINERGY BARRA CHOCO MANI 18G/24U/12D</t>
+  </si>
+  <si>
+    <t>80000158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80000158       </t>
+  </si>
+  <si>
+    <t>GALL BISCOLATA MOOD RELL CHOC 25G/24U/6D</t>
+  </si>
+  <si>
+    <t>80000155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80000155       </t>
+  </si>
+  <si>
+    <t>BISCOLATA CARAM CUBIET CHOCO 20G/24U/12D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">047329              </t>
+  </si>
+  <si>
+    <t>MEZCLA LACTEA NUTRILAC CJ*480GR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,12 +142,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -181,7 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -203,9 +233,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,19 +581,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61E602C8-8B61-412A-B23C-0E4D70479E60}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="59.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="10"/>
+    <col min="1" max="1" width="13.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -587,20 +614,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="6">
+        <v>50001179</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7">
-        <v>0.94599999999999995</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -608,163 +635,193 @@
         <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>50001045</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="7">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.48</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="5"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="5"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="5"/>
-      <c r="D11" s="11"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="5"/>
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="5"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="5"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="5"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="5"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="5"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="5"/>
-      <c r="D18" s="11"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="5"/>
-      <c r="D19" s="11"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="5"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="5"/>
-      <c r="D21" s="11"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="5"/>
-      <c r="D22" s="11"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="5"/>
-      <c r="D23" s="11"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="5"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="5"/>
-      <c r="D25" s="11"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="5"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>